<commit_message>
add input and filter
</commit_message>
<xml_diff>
--- a/week-2/Excel Adventures/demo.xlsx
+++ b/week-2/Excel Adventures/demo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -39,6 +39,15 @@
   </x:si>
   <x:si>
     <x:t>(123) IAM ACAT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>def</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Amy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>767-154-6844</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -931,6 +940,22 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
+    <x:row r="6" spans="1:2">
+      <x:c r="A6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2">
+      <x:c r="A7" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>